<commit_message>
Adicionando a especificacao do caso de uso cadastrar funcionario
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -760,7 +760,7 @@
         <v>34</v>
       </c>
       <c r="E18" s="15"/>
-      <c r="F18" s="12"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="9"/>
       <c r="H18" s="13"/>
       <c r="I18" s="14"/>

</xml_diff>

<commit_message>
Adicionando as tarefas e os modulos
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Modelo Relacional</t>
   </si>
@@ -93,65 +93,101 @@
     <t>Diagrama de Classes</t>
   </si>
   <si>
-    <t>barato</t>
-  </si>
-  <si>
-    <t>manhice</t>
-  </si>
-  <si>
-    <t>mondlane</t>
-  </si>
-  <si>
-    <t>mazivila</t>
-  </si>
-  <si>
-    <t>nhatumbo</t>
-  </si>
-  <si>
-    <t>chume</t>
-  </si>
-  <si>
-    <t>bucene</t>
-  </si>
-  <si>
-    <t>Pedir de transferência de aluno</t>
-  </si>
-  <si>
-    <t>Criar turmas</t>
-  </si>
-  <si>
-    <t>Cadastrar funcionários da escola</t>
-  </si>
-  <si>
-    <t>Cadastrar disciplina</t>
-  </si>
-  <si>
-    <t>Distribuir professores por classe e disciplina</t>
-  </si>
-  <si>
-    <t>Elaboração de horário para as turmas</t>
-  </si>
-  <si>
-    <t>pedir vaga</t>
-  </si>
-  <si>
-    <t>Transferir o aluno interno</t>
-  </si>
-  <si>
-    <t>Mockup</t>
-  </si>
-  <si>
     <t>Diagrama de Actividades</t>
   </si>
   <si>
-    <t>efectuado</t>
+    <t>Diagrama de Estados</t>
+  </si>
+  <si>
+    <t>Registar Candidatos a Aluno</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Registar Disciplinas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Listar Candidatos Registados</t>
+  </si>
+  <si>
+    <t>Listar Candidatos Pre-Matriculados</t>
+  </si>
+  <si>
+    <t>Listar Alunos Matriculados</t>
+  </si>
+  <si>
+    <t>Login Pre-Matricula</t>
+  </si>
+  <si>
+    <t>Login Principal</t>
+  </si>
+  <si>
+    <t>Recuperacao de Senha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concluido </t>
+  </si>
+  <si>
+    <t>Deve Ser melhorado</t>
+  </si>
+  <si>
+    <t>Por Fazer</t>
+  </si>
+  <si>
+    <t>Cores</t>
+  </si>
+  <si>
+    <t>Significado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Mockup</t>
+  </si>
+  <si>
+    <t>Conexao com Base de Dados</t>
+  </si>
+  <si>
+    <t>Codigo (WEB)</t>
+  </si>
+  <si>
+    <t>Candido Barato</t>
+  </si>
+  <si>
+    <t>Claudio Bucene</t>
+  </si>
+  <si>
+    <t>Absalao Nelio</t>
+  </si>
+  <si>
+    <t>Eurico Mazivila</t>
+  </si>
+  <si>
+    <t>Paulo Modlane</t>
+  </si>
+  <si>
+    <t>Ricardo Manhice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +229,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -214,11 +265,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
       </patternFill>
     </fill>
     <fill>
@@ -239,18 +285,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -263,24 +297,40 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -288,43 +338,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="10"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Accent2" xfId="4" builtinId="33"/>
-    <cellStyle name="Accent3" xfId="5" builtinId="37"/>
-    <cellStyle name="Accent5" xfId="6" builtinId="45"/>
+  <cellStyles count="11">
+    <cellStyle name="40% - Accent6" xfId="10" builtinId="51"/>
+    <cellStyle name="60% - Accent2" xfId="8" builtinId="36"/>
+    <cellStyle name="60% - Accent5" xfId="9" builtinId="48"/>
+    <cellStyle name="Accent1" xfId="7" builtinId="29"/>
+    <cellStyle name="Accent3" xfId="4" builtinId="37"/>
+    <cellStyle name="Accent5" xfId="5" builtinId="45"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,277 +708,639 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N34"/>
+  <dimension ref="A2:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="40.9453125" customWidth="1"/>
+    <col min="2" max="3" width="30.83984375" customWidth="1"/>
     <col min="4" max="4" width="40.47265625" customWidth="1"/>
     <col min="5" max="5" width="22.83984375" customWidth="1"/>
     <col min="6" max="6" width="24.3671875" customWidth="1"/>
-    <col min="7" max="11" width="20.578125" customWidth="1"/>
+    <col min="7" max="9" width="20.578125" customWidth="1"/>
+    <col min="10" max="10" width="40.578125" customWidth="1"/>
+    <col min="11" max="11" width="20.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="E2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="E3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="D5" s="7" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="C5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="D5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="E5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="F5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="6"/>
+      <c r="B26" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="7"/>
+      <c r="B27" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="8"/>
+      <c r="B28" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D6" s="6" t="s">
+      <c r="I33" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A35" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D7" s="6" t="s">
+      <c r="B35" s="15"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="17"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A36" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D8" s="6" t="s">
+      <c r="B36" s="16"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A37" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A38" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="15"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A39" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D9" s="6" t="s">
+      <c r="B39" s="14"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="16"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="15"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="17"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D10" s="6" t="s">
+      <c r="B41" s="16"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A42" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A43" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D11" s="6" t="s">
+      <c r="B43" s="2"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="15"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A44" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D12" s="6" t="s">
+      <c r="B44" s="14"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="16"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A45" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="D16" s="6" t="s">
+      <c r="B45" s="15"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="17"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A46" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="D17" s="6" t="s">
+      <c r="B46" s="16"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A47" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="D18" s="6" t="s">
+      <c r="B47" s="17"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A48" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="D19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="11"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="D20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="13"/>
-      <c r="D21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="D22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="13"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="D24" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="E25" t="s">
+      <c r="B48" s="2"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="15"/>
+    </row>
+    <row r="49" spans="1:2" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="2"/>
+      <c r="B52" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A53" s="14"/>
+      <c r="B53" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A54" s="15"/>
+      <c r="B54" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="16"/>
+      <c r="B55" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="17"/>
+      <c r="B56" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="18"/>
+      <c r="B58" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B66" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="E27" s="3" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="C68" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="D68" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="D28" s="1" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="D29" s="2" t="s">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="D30" s="2" t="s">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="D31" s="2" t="s">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="D32" s="2" t="s">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D33" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D34" s="2" t="s">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>